<commit_message>
add feature on delete and fixing some bugs
</commit_message>
<xml_diff>
--- a/public/template/guest_upload/qr_data_template_example.xlsx
+++ b/public/template/guest_upload/qr_data_template_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\personal\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA323551-327C-44DD-8681-246689833198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{965D2A0A-6C47-4BCA-A64B-84A0F8B9ED71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11295" xr2:uid="{F0E48976-7656-4FBB-B39B-6924DC478CF8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F0E48976-7656-4FBB-B39B-6924DC478CF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -98,7 +98,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -438,35 +438,35 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>